<commit_message>
update few error correction
</commit_message>
<xml_diff>
--- a/keywords.xlsx
+++ b/keywords.xlsx
@@ -2,9 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="600" firstSheet="0" activeTab="6" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Monday" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,7 +15,7 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sunday" sheetId="7" state="visible" r:id="rId7"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -56,7 +55,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -419,13 +418,18 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A14" sqref="A1:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="29.7109375" customWidth="1" min="1" max="1"/>
+    <col width="45.5703125" customWidth="1" min="2" max="2"/>
+    <col width="42.85546875" customWidth="1" min="3" max="3"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
@@ -469,6 +473,69 @@
       <c r="A5" t="inlineStr">
         <is>
           <t>Bombay</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Machine </t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Climate </t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cute cat </t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Web </t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Top travel </t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Funny </t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cloud </t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">IELTS </t>
         </is>
       </c>
     </row>
@@ -483,10 +550,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" sqref="A1:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -511,28 +578,91 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Football</t>
+          <t>Dhaka</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Paper</t>
+          <t>University</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Knife</t>
+          <t>Cricket</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Coffee</t>
+          <t>Bombay</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Machine </t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Climate </t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cute cat </t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Web </t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Top travel </t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Funny </t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cloud </t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">IELTS </t>
         </is>
       </c>
     </row>
@@ -547,10 +677,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" sqref="A1:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -575,30 +705,91 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Book</t>
+          <t>Dhaka</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Shop</t>
+          <t>University</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Laptop</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr"/>
+          <t>Cricket</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Phone</t>
+          <t>Bombay</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Machine </t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Climate </t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cute cat </t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Web </t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Top travel </t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Funny </t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cloud </t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">IELTS </t>
         </is>
       </c>
     </row>
@@ -613,10 +804,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" sqref="A1:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -641,28 +832,221 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Music</t>
+          <t>Dhaka</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>বিশ্ববিদ্যালয়, ঢাকা, বাংলাদেশ</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>ঢাকা</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Dance</t>
+          <t>University</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>দ্য ইন্টারন্যাশনাল ইউনিভার্সিটি অফ স্কলারস — বেসরকারি বিশ্ববিদ্যালয়, ঢাকা, বাংলাদেশ</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>university</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Photography</t>
+          <t>Cricket</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>আইসিসি ক্রিকেট বিশ্ব কাপ — ক্রিকেট লীগ</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>crickex</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Painting</t>
+          <t>Bombay</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>বোম্বে সুইটস এন্ড চানাচুর · chawlk, Circuler Rd, ঢাকা</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>Bombay</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Machine </t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>মাচাইন গুন কেলি — আমেরিকান র‍্যাপার</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>machine gun</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Climate </t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>climate change paragraph 150 words pdf</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>climate change</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cute cat </t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>cute cat profile picture</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>cute cat pic</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best </t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>best football player in the world</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>Best Buy</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Web </t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>web push notifications</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>web do</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Top travel </t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>top travel agencies in the world</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>top travel movies</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Funny </t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>funny birthday wishes for best friend</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>funny pic</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cloud </t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>cloud meaning in bengali</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>cloud ai</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">IELTS </t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>ielts listening practice</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>ielts liz</t>
         </is>
       </c>
     </row>
@@ -677,10 +1061,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" sqref="A1:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -705,28 +1089,91 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Holiday</t>
+          <t>Dhaka</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Vacation</t>
+          <t>University</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Adventure</t>
+          <t>Cricket</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Tourism</t>
+          <t>Bombay</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Machine </t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Climate </t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cute cat </t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Web </t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Top travel </t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Funny </t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cloud </t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">IELTS </t>
         </is>
       </c>
     </row>
@@ -741,10 +1188,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A1" sqref="A1:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -769,28 +1216,91 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Study</t>
+          <t>Dhaka</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Work</t>
+          <t>University</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Project</t>
+          <t>Cricket</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Exercise</t>
+          <t>Bombay</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Machine </t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Climate </t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cute cat </t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Web </t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Top travel </t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Funny </t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cloud </t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">IELTS </t>
         </is>
       </c>
     </row>
@@ -805,10 +1315,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -833,28 +1343,91 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Rest</t>
+          <t>Dhaka</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Family</t>
+          <t>University</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Fun</t>
+          <t>Cricket</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Relax</t>
+          <t>Bombay</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Machine </t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Climate </t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cute cat </t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Best </t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Web </t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Top travel </t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Funny </t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t xml:space="preserve">Cloud </t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t xml:space="preserve">IELTS </t>
         </is>
       </c>
     </row>

</xml_diff>